<commit_message>
budget, images, and past event update
</commit_message>
<xml_diff>
--- a/budget/budget2024.xlsx
+++ b/budget/budget2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felicia/Desktop/lille_kat/lillekat.github.io/budget/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B859A82-EACA-EA4E-8E77-ACD5A441E1BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4CF50A-0C6F-1847-9DAC-1AE12C61E54B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" activeTab="2" xr2:uid="{D1CCE3FA-2749-BB47-B79F-67BB4C56A698}"/>
+    <workbookView xWindow="2400" yWindow="940" windowWidth="26100" windowHeight="11720" activeTab="2" xr2:uid="{D1CCE3FA-2749-BB47-B79F-67BB4C56A698}"/>
   </bookViews>
   <sheets>
     <sheet name="2022" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="57">
   <si>
     <t>Lillekat 2022 budget</t>
   </si>
@@ -195,6 +195,18 @@
   </si>
   <si>
     <t>penge på snacks</t>
+  </si>
+  <si>
+    <t>Lillekat2024-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skinke </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alternatively: </t>
+  </si>
+  <si>
+    <t>nr til besilling</t>
   </si>
 </sst>
 </file>
@@ -611,7 +623,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -677,6 +689,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -704,7 +717,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1039,26 +1052,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="52"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
+      <c r="A2" s="53"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
     </row>
     <row r="3" spans="1:8" ht="28" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
@@ -1243,10 +1256,10 @@
     </row>
     <row r="10" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="53" t="s">
+      <c r="B11" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="54"/>
+      <c r="C11" s="55"/>
       <c r="D11" s="22" t="s">
         <v>17</v>
       </c>
@@ -1387,10 +1400,10 @@
     </row>
     <row r="23" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="53" t="s">
+      <c r="B24" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="54"/>
+      <c r="C24" s="55"/>
       <c r="D24" s="22" t="s">
         <v>17</v>
       </c>
@@ -1541,8 +1554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B219F9F2-A4CC-AD4F-A3F1-917E919B80E2}">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView zoomScale="114" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="A5" zoomScale="114" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1561,26 +1574,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="52"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
+      <c r="A2" s="53"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
     </row>
     <row r="3" spans="1:12" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1607,10 +1620,10 @@
       <c r="H3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="57" t="s">
+      <c r="K3" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="L3" s="58"/>
+      <c r="L3" s="59"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -1636,10 +1649,10 @@
         <f>E4*F4</f>
         <v>4500</v>
       </c>
-      <c r="K4" s="55" t="s">
+      <c r="K4" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="56"/>
+      <c r="L4" s="57"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
@@ -1826,17 +1839,17 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="K12" s="55" t="s">
+      <c r="K12" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="L12" s="56"/>
+      <c r="L12" s="57"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B13" s="53" t="s">
+      <c r="B13" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="54"/>
-      <c r="D13" s="59"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="60"/>
       <c r="K13" s="44" t="s">
         <v>33</v>
       </c>
@@ -2014,10 +2027,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3C72BB-923F-DB4A-A4B9-C9C78647B110}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2026,31 +2039,32 @@
     <col min="2" max="2" width="12.1640625" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" customWidth="1"/>
     <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="52"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-    </row>
-    <row r="3" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="53"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+    </row>
+    <row r="3" spans="1:11" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
@@ -2075,10 +2089,10 @@
       <c r="H3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="57" t="s">
+      <c r="J3" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="58"/>
+      <c r="K3" s="59"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -2093,16 +2107,16 @@
       <c r="D4">
         <v>61</v>
       </c>
-      <c r="E4" s="60">
+      <c r="E4" s="51">
         <v>1475</v>
       </c>
       <c r="F4" s="32"/>
       <c r="G4" s="33"/>
       <c r="H4" s="34"/>
-      <c r="J4" s="55" t="s">
+      <c r="J4" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="56"/>
+      <c r="K4" s="57"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
@@ -2112,9 +2126,16 @@
         <v>45345</v>
       </c>
       <c r="C5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="33"/>
+      <c r="E5" s="4">
+        <v>1495</v>
+      </c>
+      <c r="F5" s="32">
+        <f>D21</f>
+        <v>2609</v>
+      </c>
+      <c r="G5" s="33">
+        <v>50</v>
+      </c>
       <c r="H5" s="34"/>
       <c r="J5" s="44" t="s">
         <v>24</v>
@@ -2214,7 +2235,7 @@
       </c>
       <c r="E10" s="21">
         <f>SUM(E4:E9)</f>
-        <v>1475</v>
+        <v>2970</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
@@ -2243,11 +2264,243 @@
       <c r="H11" s="21"/>
     </row>
     <row r="12" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B14" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="55"/>
+      <c r="D14" s="60"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B15" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="23">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" s="24">
+        <f>B16*110</f>
+        <v>550</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="23">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17" s="24">
+        <f>B17*139</f>
+        <v>556</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="23">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>10</v>
+      </c>
+      <c r="D18" s="24">
+        <f>B18*129</f>
+        <v>516</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="23">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>12</v>
+      </c>
+      <c r="D19" s="24">
+        <f>B19*129</f>
+        <v>387</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="23">
+        <v>4</v>
+      </c>
+      <c r="C20" s="25">
+        <v>24</v>
+      </c>
+      <c r="D20" s="24">
+        <f>B20*150</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="29">
+        <f>SUM(B16:B20)</f>
+        <v>20</v>
+      </c>
+      <c r="C21" s="30"/>
+      <c r="D21" s="31">
+        <f>SUM(D16:D20)</f>
+        <v>2609</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="55"/>
+      <c r="D24" s="60"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B25" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="23">
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" s="24">
+        <f>B26*65</f>
+        <v>325</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="23">
+        <v>5</v>
+      </c>
+      <c r="C27">
+        <v>5</v>
+      </c>
+      <c r="D27" s="24">
+        <f>B27*79</f>
+        <v>395</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="23">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>10</v>
+      </c>
+      <c r="D28" s="24">
+        <f>B28*75</f>
+        <v>375</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="23">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <v>12</v>
+      </c>
+      <c r="D29" s="24">
+        <f>B29*75</f>
+        <v>375</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="23">
+        <v>5</v>
+      </c>
+      <c r="C30" s="25">
+        <v>24</v>
+      </c>
+      <c r="D30" s="24">
+        <f>B30*85</f>
+        <v>425</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="29">
+        <f>SUM(B26:B30)</f>
+        <v>25</v>
+      </c>
+      <c r="C31" s="30"/>
+      <c r="D31" s="31">
+        <f>SUM(D26:D30)</f>
+        <v>1895</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="61" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>26786171</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="A1:H2"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="J4:K4"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B24:D24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
budget and kattepasser101 update
</commit_message>
<xml_diff>
--- a/budget/budget2024.xlsx
+++ b/budget/budget2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felicia/Desktop/lille_kat/lillekat.github.io/budget/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4CF50A-0C6F-1847-9DAC-1AE12C61E54B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48629294-B407-1642-B385-95AFE732D760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2400" yWindow="940" windowWidth="26100" windowHeight="11720" activeTab="2" xr2:uid="{D1CCE3FA-2749-BB47-B79F-67BB4C56A698}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="57">
   <si>
     <t>Lillekat 2022 budget</t>
   </si>
@@ -203,10 +203,10 @@
     <t xml:space="preserve">Skinke </t>
   </si>
   <si>
-    <t xml:space="preserve">Alternatively: </t>
-  </si>
-  <si>
     <t>nr til besilling</t>
+  </si>
+  <si>
+    <t>penge på pizza</t>
   </si>
 </sst>
 </file>
@@ -623,7 +623,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -717,7 +717,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -2027,10 +2026,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3C72BB-923F-DB4A-A4B9-C9C78647B110}">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2039,10 +2038,12 @@
     <col min="2" max="2" width="12.1640625" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" customWidth="1"/>
     <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="52" t="s">
         <v>46</v>
       </c>
@@ -2052,9 +2053,8 @@
       <c r="E1" s="52"/>
       <c r="F1" s="52"/>
       <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="53"/>
       <c r="B2" s="53"/>
       <c r="C2" s="53"/>
@@ -2062,9 +2062,8 @@
       <c r="E2" s="53"/>
       <c r="F2" s="53"/>
       <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-    </row>
-    <row r="3" spans="1:11" ht="25" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:10" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
@@ -2080,21 +2079,18 @@
       <c r="E3" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="F3" s="17" t="s">
-        <v>13</v>
+      <c r="F3" s="49" t="s">
+        <v>56</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="58" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="59"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J3" s="59"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>48</v>
       </c>
@@ -2110,15 +2106,17 @@
       <c r="E4" s="51">
         <v>1475</v>
       </c>
-      <c r="F4" s="32"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="34"/>
-      <c r="J4" s="56" t="s">
+      <c r="F4" s="51"/>
+      <c r="G4" s="33">
+        <f>F4+E4</f>
+        <v>1475</v>
+      </c>
+      <c r="I4" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="57"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J4" s="57"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -2129,22 +2127,21 @@
       <c r="E5" s="4">
         <v>1495</v>
       </c>
-      <c r="F5" s="32">
-        <f>D21</f>
+      <c r="F5" s="4">
         <v>2609</v>
       </c>
       <c r="G5" s="33">
-        <v>50</v>
-      </c>
-      <c r="H5" s="34"/>
-      <c r="J5" s="44" t="s">
+        <f t="shared" ref="G5:G9" si="0">F5+E5</f>
+        <v>4104</v>
+      </c>
+      <c r="I5" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="K5" s="48">
+      <c r="J5" s="48">
         <v>12000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>49</v>
       </c>
@@ -2153,17 +2150,19 @@
       </c>
       <c r="C6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="34"/>
-      <c r="J6" s="44" t="s">
+      <c r="F6" s="4"/>
+      <c r="G6" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="K6" s="48">
+      <c r="J6" s="48">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>50</v>
       </c>
@@ -2172,17 +2171,19 @@
       </c>
       <c r="C7" s="4"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="34"/>
-      <c r="J7" s="44" t="s">
+      <c r="F7" s="4"/>
+      <c r="G7" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="K7" s="48">
+      <c r="J7" s="48">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>51</v>
       </c>
@@ -2191,17 +2192,19 @@
       </c>
       <c r="C8" s="4"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="34"/>
-      <c r="J8" s="47" t="s">
+      <c r="F8" s="4"/>
+      <c r="G8" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="K8" s="41">
+      <c r="J8" s="41">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>47</v>
       </c>
@@ -2210,17 +2213,19 @@
       </c>
       <c r="C9" s="4"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="34"/>
-      <c r="J9" s="47" t="s">
+      <c r="F9" s="4"/>
+      <c r="G9" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="K9" s="41">
+      <c r="J9" s="41">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>14</v>
       </c>
@@ -2237,41 +2242,40 @@
         <f>SUM(E4:E9)</f>
         <v>2970</v>
       </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21">
-        <f>SUM(H4:H9)</f>
-        <v>0</v>
-      </c>
-      <c r="J10" s="40" t="s">
+      <c r="F10" s="21">
+        <f>SUM(F4:F9)</f>
+        <v>2609</v>
+      </c>
+      <c r="G10" s="21">
+        <f>E10+F10</f>
+        <v>5579</v>
+      </c>
+      <c r="I10" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="K10" s="46">
-        <f>SUM(K5:K9)</f>
+      <c r="J10" s="46">
+        <f>SUM(J5:J9)</f>
         <v>12000</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
-        <v>20</v>
-      </c>
+    <row r="11" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="20"/>
       <c r="B11" s="20"/>
       <c r="C11" s="35"/>
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
-      <c r="F11" s="21"/>
+      <c r="F11" s="20"/>
       <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-    </row>
-    <row r="12" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:10" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14" s="54" t="s">
         <v>53</v>
       </c>
       <c r="C14" s="55"/>
       <c r="D14" s="60"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B15" s="22" t="s">
         <v>38</v>
       </c>
@@ -2281,9 +2285,8 @@
       <c r="D15" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="50" t="s">
         <v>40</v>
       </c>
@@ -2373,134 +2376,22 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="54" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="55"/>
-      <c r="D24" s="60"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="22" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="23">
-        <v>5</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26" s="24">
-        <f>B26*65</f>
-        <v>325</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" s="23">
-        <v>5</v>
-      </c>
-      <c r="C27">
-        <v>5</v>
-      </c>
-      <c r="D27" s="24">
-        <f>B27*79</f>
-        <v>395</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" s="23">
-        <v>5</v>
-      </c>
-      <c r="C28">
-        <v>10</v>
-      </c>
-      <c r="D28" s="24">
-        <f>B28*75</f>
-        <v>375</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="50" t="s">
-        <v>54</v>
-      </c>
-      <c r="B29" s="23">
-        <v>5</v>
-      </c>
-      <c r="C29">
-        <v>12</v>
-      </c>
-      <c r="D29" s="24">
-        <f>B29*75</f>
-        <v>375</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="50" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="23">
-        <v>5</v>
-      </c>
-      <c r="C30" s="25">
-        <v>24</v>
-      </c>
-      <c r="D30" s="24">
-        <f>B30*85</f>
-        <v>425</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="B31" s="29">
-        <f>SUM(B26:B30)</f>
-        <v>25</v>
-      </c>
-      <c r="C31" s="30"/>
-      <c r="D31" s="31">
-        <f>SUM(D26:D30)</f>
-        <v>1895</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="61" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34">
+      <c r="A26">
         <v>26786171</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
+  <mergeCells count="4">
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B24:D24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
image, index, and kattepasser101 basecamp update
</commit_message>
<xml_diff>
--- a/budget/budget2024.xlsx
+++ b/budget/budget2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felicia/Desktop/lille_kat/lillekat.github.io/budget/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48629294-B407-1642-B385-95AFE732D760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F0B364-24F9-AB4C-B9D2-0690B32A41F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2400" yWindow="940" windowWidth="26100" windowHeight="11720" activeTab="2" xr2:uid="{D1CCE3FA-2749-BB47-B79F-67BB4C56A698}"/>
   </bookViews>
@@ -2028,8 +2028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3C72BB-923F-DB4A-A4B9-C9C78647B110}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2123,7 +2123,12 @@
       <c r="B5" s="7">
         <v>45345</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="4">
+        <v>39</v>
+      </c>
+      <c r="D5">
+        <v>110</v>
+      </c>
       <c r="E5" s="4">
         <v>1495</v>
       </c>
@@ -2232,11 +2237,11 @@
       <c r="B10" s="20"/>
       <c r="C10" s="35">
         <f>SUM(C4:C9)</f>
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="D10" s="20">
         <f>SUM(D4:D9)</f>
-        <v>61</v>
+        <v>171</v>
       </c>
       <c r="E10" s="21">
         <f>SUM(E4:E9)</f>

</xml_diff>

<commit_message>
past events and index update
</commit_message>
<xml_diff>
--- a/budget/budget2024.xlsx
+++ b/budget/budget2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felicia/Desktop/lille_kat/lillekat.github.io/budget/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F0B364-24F9-AB4C-B9D2-0690B32A41F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF1947A-B438-2647-8F36-6A8C2F9BB064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2400" yWindow="940" windowWidth="26100" windowHeight="11720" activeTab="2" xr2:uid="{D1CCE3FA-2749-BB47-B79F-67BB4C56A698}"/>
   </bookViews>
@@ -1553,8 +1553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B219F9F2-A4CC-AD4F-A3F1-917E919B80E2}">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="114" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView zoomScale="114" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2028,8 +2028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3C72BB-923F-DB4A-A4B9-C9C78647B110}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
event update and past event date correction
</commit_message>
<xml_diff>
--- a/budget/budget2024.xlsx
+++ b/budget/budget2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felicia/Desktop/lille_kat/lillekat.github.io/budget/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF1947A-B438-2647-8F36-6A8C2F9BB064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C75FDB-C0AF-5441-8539-FE76F93C0DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="940" windowWidth="26100" windowHeight="11720" activeTab="2" xr2:uid="{D1CCE3FA-2749-BB47-B79F-67BB4C56A698}"/>
+    <workbookView xWindow="2400" yWindow="940" windowWidth="26100" windowHeight="8900" activeTab="2" xr2:uid="{D1CCE3FA-2749-BB47-B79F-67BB4C56A698}"/>
   </bookViews>
   <sheets>
     <sheet name="2022" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="57">
   <si>
     <t>Lillekat 2022 budget</t>
   </si>
@@ -179,15 +179,9 @@
     <t>Lillekat 2024 budget</t>
   </si>
   <si>
-    <t>Lillekat2024-06</t>
-  </si>
-  <si>
     <t>Lillekat2024-01</t>
   </si>
   <si>
-    <t>Lillekat2024-03</t>
-  </si>
-  <si>
     <t>Lillekat2024-04</t>
   </si>
   <si>
@@ -207,6 +201,12 @@
   </si>
   <si>
     <t>penge på pizza</t>
+  </si>
+  <si>
+    <t>Lillekat2024-03 Novo sponsoreret</t>
+  </si>
+  <si>
+    <t>Lillekat2024 D-Pop</t>
   </si>
 </sst>
 </file>
@@ -2028,14 +2028,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3C72BB-923F-DB4A-A4B9-C9C78647B110}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.1640625" customWidth="1"/>
     <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" customWidth="1"/>
     <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5" customWidth="1"/>
@@ -2077,10 +2078,10 @@
         <v>3</v>
       </c>
       <c r="E3" s="49" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F3" s="49" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G3" s="17" t="s">
         <v>18</v>
@@ -2092,7 +2093,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="2">
         <v>45331</v>
@@ -2148,18 +2149,24 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B6" s="7">
         <v>45366</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="33">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="C6" s="4">
+        <v>40</v>
+      </c>
+      <c r="D6">
+        <v>52</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="33"/>
       <c r="I6" s="44" t="s">
         <v>27</v>
       </c>
@@ -2169,17 +2176,19 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B7" s="7">
         <v>45387</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="E7" s="4">
+        <v>3200</v>
+      </c>
       <c r="F7" s="4"/>
       <c r="G7" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3200</v>
       </c>
       <c r="I7" s="44" t="s">
         <v>27</v>
@@ -2190,7 +2199,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B8" s="7">
         <v>45401</v>
@@ -2211,7 +2220,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B9" s="7">
         <v>45415</v>
@@ -2237,15 +2246,15 @@
       <c r="B10" s="20"/>
       <c r="C10" s="35">
         <f>SUM(C4:C9)</f>
-        <v>51</v>
+        <v>91</v>
       </c>
       <c r="D10" s="20">
         <f>SUM(D4:D9)</f>
-        <v>171</v>
+        <v>223</v>
       </c>
       <c r="E10" s="21">
         <f>SUM(E4:E9)</f>
-        <v>2970</v>
+        <v>6170</v>
       </c>
       <c r="F10" s="21">
         <f>SUM(F4:F9)</f>
@@ -2253,7 +2262,7 @@
       </c>
       <c r="G10" s="21">
         <f>E10+F10</f>
-        <v>5579</v>
+        <v>8779</v>
       </c>
       <c r="I10" s="40" t="s">
         <v>14</v>
@@ -2275,7 +2284,7 @@
     <row r="12" spans="1:10" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14" s="54" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C14" s="55"/>
       <c r="D14" s="60"/>
@@ -2338,7 +2347,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="50" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B19" s="23">
         <v>3</v>
@@ -2383,7 +2392,7 @@
     <row r="22" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="36" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
index and attendees 04 update
</commit_message>
<xml_diff>
--- a/budget/budget2024.xlsx
+++ b/budget/budget2024.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felicia/Desktop/lille_kat/lillekat.github.io/budget/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felicia/Desktop/lillekat.github.io/budget/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E3E498-951C-664A-A048-1A2BBAA728D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A1AE719-EA35-2348-91FC-4101F41C3515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2400" yWindow="940" windowWidth="26100" windowHeight="13880" activeTab="2" xr2:uid="{D1CCE3FA-2749-BB47-B79F-67BB4C56A698}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="58">
   <si>
     <t>Lillekat 2022 budget</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>Lillekat2024 D-Pop</t>
+  </si>
+  <si>
+    <t>$</t>
   </si>
 </sst>
 </file>
@@ -2029,7 +2032,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2181,7 +2184,12 @@
       <c r="B7" s="7">
         <v>45387</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="4">
+        <v>22</v>
+      </c>
+      <c r="D7">
+        <v>29</v>
+      </c>
       <c r="E7" s="4">
         <v>3233</v>
       </c>
@@ -2247,11 +2255,11 @@
       <c r="B10" s="20"/>
       <c r="C10" s="35">
         <f>SUM(C4:C9)</f>
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="D10" s="20">
         <f>SUM(D4:D9)</f>
-        <v>223</v>
+        <v>252</v>
       </c>
       <c r="E10" s="21">
         <f>SUM(E4:E9)</f>
@@ -2316,7 +2324,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="50" t="s">
         <v>41</v>
       </c>
@@ -2330,8 +2338,11 @@
         <f>B17*139</f>
         <v>556</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="50" t="s">
         <v>42</v>
       </c>
@@ -2346,7 +2357,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="50" t="s">
         <v>52</v>
       </c>
@@ -2361,7 +2372,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="50" t="s">
         <v>44</v>
       </c>
@@ -2376,7 +2387,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
         <v>18</v>
       </c>
@@ -2390,13 +2401,13 @@
         <v>2609</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="36" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>26786171</v>
       </c>

</xml_diff>

<commit_message>
readit template grammatik og kattepasser101 basecamp update
</commit_message>
<xml_diff>
--- a/budget/budget2024.xlsx
+++ b/budget/budget2024.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felicia/Desktop/lillekat.github.io/budget/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A1AE719-EA35-2348-91FC-4101F41C3515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91BA0D5-D000-F944-AB99-905404EE214A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2400" yWindow="940" windowWidth="26100" windowHeight="13880" activeTab="2" xr2:uid="{D1CCE3FA-2749-BB47-B79F-67BB4C56A698}"/>
   </bookViews>
@@ -2031,8 +2031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3C72BB-923F-DB4A-A4B9-C9C78647B110}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2122,7 +2122,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="B5" s="7">
         <v>45345</v>

</xml_diff>

<commit_message>
budget, upcoming events, and past events update
</commit_message>
<xml_diff>
--- a/budget/budget2024.xlsx
+++ b/budget/budget2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felicia/Desktop/lillekat.github.io/budget/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91BA0D5-D000-F944-AB99-905404EE214A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1740AB04-0AD1-DD41-B2D7-7F093DFE2495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="940" windowWidth="26100" windowHeight="13880" activeTab="2" xr2:uid="{D1CCE3FA-2749-BB47-B79F-67BB4C56A698}"/>
+    <workbookView xWindow="5940" yWindow="500" windowWidth="22860" windowHeight="9800" activeTab="2" xr2:uid="{D1CCE3FA-2749-BB47-B79F-67BB4C56A698}"/>
   </bookViews>
   <sheets>
     <sheet name="2022" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="58">
   <si>
     <t>Lillekat 2022 budget</t>
   </si>
@@ -209,7 +209,7 @@
     <t>Lillekat2024 D-Pop</t>
   </si>
   <si>
-    <t>$</t>
+    <t xml:space="preserve">det blev faktisk kun 1670 </t>
   </si>
 </sst>
 </file>
@@ -220,7 +220,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;kr.&quot;_-;\-* #,##0.00\ &quot;kr.&quot;_-;_-* &quot;-&quot;??\ &quot;kr.&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;kr.&quot;"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -288,8 +288,22 @@
       <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Georgia Pro"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -332,8 +346,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="25">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -621,12 +641,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -693,6 +726,18 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -718,6 +763,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1054,26 +1108,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="53"/>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
+      <c r="A2" s="63"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
     </row>
     <row r="3" spans="1:8" ht="28" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
@@ -1258,10 +1312,10 @@
     </row>
     <row r="10" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="55"/>
+      <c r="C11" s="65"/>
       <c r="D11" s="22" t="s">
         <v>17</v>
       </c>
@@ -1402,10 +1456,10 @@
     </row>
     <row r="23" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="54" t="s">
+      <c r="B24" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="55"/>
+      <c r="C24" s="65"/>
       <c r="D24" s="22" t="s">
         <v>17</v>
       </c>
@@ -1576,26 +1630,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="53"/>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
+      <c r="A2" s="63"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
     </row>
     <row r="3" spans="1:12" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1622,10 +1676,10 @@
       <c r="H3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="58" t="s">
+      <c r="K3" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="L3" s="59"/>
+      <c r="L3" s="69"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -1651,10 +1705,10 @@
         <f>E4*F4</f>
         <v>4500</v>
       </c>
-      <c r="K4" s="56" t="s">
+      <c r="K4" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="57"/>
+      <c r="L4" s="67"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
@@ -1841,17 +1895,17 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="K12" s="56" t="s">
+      <c r="K12" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="L12" s="57"/>
+      <c r="L12" s="67"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B13" s="54" t="s">
+      <c r="B13" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="55"/>
-      <c r="D13" s="60"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="70"/>
       <c r="K13" s="44" t="s">
         <v>33</v>
       </c>
@@ -2031,8 +2085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3C72BB-923F-DB4A-A4B9-C9C78647B110}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2043,29 +2097,29 @@
     <col min="4" max="4" width="16.83203125" customWidth="1"/>
     <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="53"/>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
+      <c r="A2" s="63"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
     </row>
     <row r="3" spans="1:10" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -2089,10 +2143,10 @@
       <c r="G3" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="58" t="s">
+      <c r="I3" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="J3" s="59"/>
+      <c r="J3" s="69"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -2115,10 +2169,10 @@
         <f>F4+E4</f>
         <v>1475</v>
       </c>
-      <c r="I4" s="56" t="s">
+      <c r="I4" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="57"/>
+      <c r="J4" s="67"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
@@ -2234,12 +2288,19 @@
       <c r="B9" s="7">
         <v>45415</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="4">
+        <v>36</v>
+      </c>
+      <c r="D9">
+        <v>60</v>
+      </c>
       <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="F9" s="4">
+        <v>1670</v>
+      </c>
       <c r="G9" s="33">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>F9+E9</f>
+        <v>1670</v>
       </c>
       <c r="I9" s="47" t="s">
         <v>23</v>
@@ -2255,11 +2316,11 @@
       <c r="B10" s="20"/>
       <c r="C10" s="35">
         <f>SUM(C4:C9)</f>
-        <v>113</v>
+        <v>149</v>
       </c>
       <c r="D10" s="20">
         <f>SUM(D4:D9)</f>
-        <v>252</v>
+        <v>312</v>
       </c>
       <c r="E10" s="21">
         <f>SUM(E4:E9)</f>
@@ -2267,11 +2328,11 @@
       </c>
       <c r="F10" s="21">
         <f>SUM(F4:F9)</f>
-        <v>2609</v>
+        <v>4279</v>
       </c>
       <c r="G10" s="21">
-        <f>E10+F10</f>
-        <v>8812</v>
+        <f>SUM(G4:G9)</f>
+        <v>10482</v>
       </c>
       <c r="I10" s="40" t="s">
         <v>14</v>
@@ -2292,11 +2353,17 @@
     </row>
     <row r="12" spans="1:10" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="54" t="s">
+      <c r="B14" s="64" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="55"/>
-      <c r="D14" s="60"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="70"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" s="72"/>
+      <c r="I14" s="73"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B15" s="22" t="s">
@@ -2308,6 +2375,16 @@
       <c r="D15" s="22" t="s">
         <v>17</v>
       </c>
+      <c r="F15" s="52"/>
+      <c r="G15" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15" s="54" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="50" t="s">
@@ -2323,8 +2400,21 @@
         <f>B16*110</f>
         <v>550</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F16" s="55" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="52">
+        <v>4</v>
+      </c>
+      <c r="H16" s="52">
+        <v>1</v>
+      </c>
+      <c r="I16" s="56">
+        <f>G16*110</f>
+        <v>440</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="50" t="s">
         <v>41</v>
       </c>
@@ -2338,11 +2428,21 @@
         <f>B17*139</f>
         <v>556</v>
       </c>
-      <c r="G17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F17" s="57" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17" s="52">
+        <v>5</v>
+      </c>
+      <c r="H17" s="52">
+        <v>5</v>
+      </c>
+      <c r="I17" s="56">
+        <f>G17*139</f>
+        <v>695</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="50" t="s">
         <v>42</v>
       </c>
@@ -2356,8 +2456,21 @@
         <f>B18*129</f>
         <v>516</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F18" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" s="52">
+        <v>5</v>
+      </c>
+      <c r="H18" s="52">
+        <v>10</v>
+      </c>
+      <c r="I18" s="56">
+        <f>G18*129</f>
+        <v>645</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="50" t="s">
         <v>52</v>
       </c>
@@ -2371,8 +2484,21 @@
         <f>B19*129</f>
         <v>387</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F19" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="G19" s="52">
+        <v>4</v>
+      </c>
+      <c r="H19" s="52">
+        <v>12</v>
+      </c>
+      <c r="I19" s="56">
+        <f>G19*129</f>
+        <v>516</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="50" t="s">
         <v>44</v>
       </c>
@@ -2386,8 +2512,21 @@
         <f>B20*150</f>
         <v>600</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F20" s="57" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="52">
+        <v>4</v>
+      </c>
+      <c r="H20" s="58">
+        <v>24</v>
+      </c>
+      <c r="I20" s="56">
+        <f>G20*150</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
         <v>18</v>
       </c>
@@ -2400,24 +2539,41 @@
         <f>SUM(D16:D20)</f>
         <v>2609</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F21" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" s="60">
+        <f>SUM(G16:G20)</f>
+        <v>22</v>
+      </c>
+      <c r="H21" s="60"/>
+      <c r="I21" s="61">
+        <f>SUM(I16:I20)</f>
+        <v>2896</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="I22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="36" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>26786171</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:G2"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="B14:D14"/>
+    <mergeCell ref="G14:I14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
index and budget update
</commit_message>
<xml_diff>
--- a/budget/budget2024.xlsx
+++ b/budget/budget2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felicia/Desktop/lillekat.github.io/budget/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felicia/Desktop/old_lillekat/budget/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF361484-E373-CB45-B758-D3095FC37C12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86701F3E-06B3-864D-AFD2-5375B5E47FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="14120" activeTab="2" xr2:uid="{D1CCE3FA-2749-BB47-B79F-67BB4C56A698}"/>
+    <workbookView xWindow="1480" yWindow="500" windowWidth="26880" windowHeight="14120" activeTab="2" xr2:uid="{D1CCE3FA-2749-BB47-B79F-67BB4C56A698}"/>
   </bookViews>
   <sheets>
     <sheet name="2022" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="88">
   <si>
     <t>Lillekat 2022 budget</t>
   </si>
@@ -304,6 +304,21 @@
   </si>
   <si>
     <t xml:space="preserve">Event Materiale </t>
+  </si>
+  <si>
+    <t>pizza 2024:06</t>
+  </si>
+  <si>
+    <t>Lillekat2024-06 normale pizzaer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nemlig snacks 06 </t>
+  </si>
+  <si>
+    <t>nemlig snacks 07</t>
+  </si>
+  <si>
+    <t>pizza 2024:07</t>
   </si>
 </sst>
 </file>
@@ -900,6 +915,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -907,9 +925,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1754,7 +1769,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B219F9F2-A4CC-AD4F-A3F1-917E919B80E2}">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView zoomScale="114" zoomScaleNormal="116" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="114" zoomScaleNormal="116" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
@@ -2227,10 +2242,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3C72BB-923F-DB4A-A4B9-C9C78647B110}">
-  <dimension ref="A1:T53"/>
+  <dimension ref="A1:AD53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2248,7 +2263,7 @@
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="76" t="s">
         <v>60</v>
       </c>
@@ -2260,7 +2275,7 @@
       <c r="G1" s="76"/>
       <c r="L1" s="65"/>
     </row>
-    <row r="2" spans="1:20" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="77"/>
       <c r="B2" s="77"/>
       <c r="C2" s="77"/>
@@ -2272,7 +2287,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:30" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
@@ -2304,13 +2319,24 @@
       <c r="N3" s="79"/>
       <c r="O3" s="84"/>
       <c r="Q3" s="52"/>
-      <c r="R3" s="85" t="s">
+      <c r="R3" s="86" t="s">
         <v>56</v>
       </c>
-      <c r="S3" s="86"/>
-      <c r="T3" s="87"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S3" s="87"/>
+      <c r="T3" s="88"/>
+      <c r="V3" s="52"/>
+      <c r="W3" s="86" t="s">
+        <v>84</v>
+      </c>
+      <c r="X3" s="87"/>
+      <c r="Y3" s="88"/>
+      <c r="AB3" s="78" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC3" s="79"/>
+      <c r="AD3" s="84"/>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>46</v>
       </c>
@@ -2354,8 +2380,27 @@
       <c r="T4" s="54" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="V4" s="52"/>
+      <c r="W4" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="X4" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y4" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB4" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC4" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD4" s="22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>50</v>
       </c>
@@ -2410,8 +2455,34 @@
         <f>R5*65</f>
         <v>260</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="V5" s="55" t="s">
+        <v>40</v>
+      </c>
+      <c r="W5" s="52">
+        <v>7</v>
+      </c>
+      <c r="X5" s="52">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="56">
+        <f>W5*75</f>
+        <v>525</v>
+      </c>
+      <c r="AA5" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB5" s="23">
+        <v>5</v>
+      </c>
+      <c r="AC5">
+        <v>1</v>
+      </c>
+      <c r="AD5" s="24">
+        <f>AB5*140</f>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>53</v>
       </c>
@@ -2464,8 +2535,34 @@
         <f>R6*79</f>
         <v>395</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="V6" s="57" t="s">
+        <v>41</v>
+      </c>
+      <c r="W6" s="52">
+        <v>7</v>
+      </c>
+      <c r="X6" s="52">
+        <v>5</v>
+      </c>
+      <c r="Y6" s="56">
+        <f>W6*85</f>
+        <v>595</v>
+      </c>
+      <c r="AA6" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB6" s="23">
+        <v>4</v>
+      </c>
+      <c r="AC6">
+        <v>5</v>
+      </c>
+      <c r="AD6" s="24">
+        <f>AB6*160</f>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>47</v>
       </c>
@@ -2512,8 +2609,34 @@
         <f>R7*75</f>
         <v>375</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="V7" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="W7" s="52">
+        <v>5</v>
+      </c>
+      <c r="X7" s="52">
+        <v>10</v>
+      </c>
+      <c r="Y7" s="56">
+        <f>W7*80</f>
+        <v>400</v>
+      </c>
+      <c r="AA7" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB7" s="23">
+        <v>3</v>
+      </c>
+      <c r="AC7">
+        <v>10</v>
+      </c>
+      <c r="AD7" s="24">
+        <f>AB7*150</f>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>54</v>
       </c>
@@ -2558,8 +2681,34 @@
         <f>R8*75</f>
         <v>300</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="V8" s="57" t="s">
+        <v>51</v>
+      </c>
+      <c r="W8" s="52">
+        <v>5</v>
+      </c>
+      <c r="X8" s="52">
+        <v>12</v>
+      </c>
+      <c r="Y8" s="56">
+        <f>W8*80</f>
+        <v>400</v>
+      </c>
+      <c r="AA8" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB8" s="23">
+        <v>3</v>
+      </c>
+      <c r="AC8">
+        <v>12</v>
+      </c>
+      <c r="AD8" s="24">
+        <f>AB8*150</f>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>48</v>
       </c>
@@ -2610,8 +2759,34 @@
         <f>R9*85</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="V9" s="57" t="s">
+        <v>44</v>
+      </c>
+      <c r="W9" s="52">
+        <v>4</v>
+      </c>
+      <c r="X9" s="58">
+        <v>24</v>
+      </c>
+      <c r="Y9" s="56">
+        <f>W9*90</f>
+        <v>360</v>
+      </c>
+      <c r="AA9" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB9" s="23">
+        <v>3</v>
+      </c>
+      <c r="AC9" s="25">
+        <v>24</v>
+      </c>
+      <c r="AD9" s="24">
+        <f>AB9*170</f>
+        <v>510</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>14</v>
       </c>
@@ -2664,8 +2839,32 @@
         <f>SUM(T5:T9)</f>
         <v>1670</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="V10" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="W10" s="60">
+        <f>SUM(W5:W9)</f>
+        <v>28</v>
+      </c>
+      <c r="X10" s="60"/>
+      <c r="Y10" s="61">
+        <f>SUM(Y5:Y9)</f>
+        <v>2280</v>
+      </c>
+      <c r="AA10" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB10" s="29">
+        <f>SUM(AB5:AB9)</f>
+        <v>18</v>
+      </c>
+      <c r="AC10" s="30"/>
+      <c r="AD10" s="31">
+        <f>SUM(AD5:AD9)</f>
+        <v>2750</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20"/>
       <c r="B11" s="20"/>
       <c r="C11" s="35"/>
@@ -2684,7 +2883,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="I12" s="44" t="s">
         <v>69</v>
       </c>
@@ -2693,7 +2892,7 @@
         <v>4279</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="I13" s="40" t="s">
         <v>14</v>
       </c>
@@ -2702,8 +2901,8 @@
         <v>10482</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="I15" s="38" t="s">
         <v>26</v>
       </c>
@@ -2712,7 +2911,7 @@
         <v>1518</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A16" s="76" t="s">
         <v>62</v>
       </c>
@@ -2760,11 +2959,20 @@
         <v>63</v>
       </c>
       <c r="B19" s="2">
-        <v>45548</v>
-      </c>
-      <c r="C19" s="4"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
+        <v>45555</v>
+      </c>
+      <c r="C19" s="4">
+        <v>64</v>
+      </c>
+      <c r="D19">
+        <v>157</v>
+      </c>
+      <c r="E19" s="51">
+        <v>3510.6</v>
+      </c>
+      <c r="F19" s="51">
+        <v>2280</v>
+      </c>
       <c r="G19" s="33"/>
       <c r="I19" s="82" t="s">
         <v>58</v>
@@ -2778,9 +2986,18 @@
       <c r="B20" s="7">
         <v>45562</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
+      <c r="C20" s="4">
+        <v>34</v>
+      </c>
+      <c r="D20">
+        <v>79</v>
+      </c>
+      <c r="E20" s="4">
+        <v>3305</v>
+      </c>
+      <c r="F20" s="4">
+        <v>2750</v>
+      </c>
       <c r="G20" s="33"/>
       <c r="I20" s="80" t="s">
         <v>25</v>
@@ -2849,19 +3066,19 @@
       <c r="B24" s="20"/>
       <c r="C24" s="35">
         <f>SUM(C19:C23)</f>
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="D24" s="20">
         <f>SUM(D19:D23)</f>
-        <v>0</v>
+        <v>236</v>
       </c>
       <c r="E24" s="21">
         <f>SUM(E19:E23)</f>
-        <v>0</v>
+        <v>6815.6</v>
       </c>
       <c r="F24" s="21">
         <f>SUM(F19:F23)</f>
-        <v>0</v>
+        <v>5030</v>
       </c>
       <c r="G24" s="21">
         <f>SUM(G19:G23)</f>
@@ -2911,7 +3128,7 @@
       </c>
       <c r="J29" s="64">
         <f>E24</f>
-        <v>0</v>
+        <v>6815.6</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
@@ -2920,7 +3137,7 @@
       </c>
       <c r="J30" s="64">
         <f>F24</f>
-        <v>0</v>
+        <v>5030</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
@@ -2941,7 +3158,7 @@
       </c>
       <c r="J33" s="66">
         <f>J27+J28+J29+J30+J31+J32</f>
-        <v>492.91</v>
+        <v>12338.51</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
@@ -2951,7 +3168,7 @@
       </c>
       <c r="J35" s="37">
         <f>J24-J33</f>
-        <v>63025.09</v>
+        <v>51179.49</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
@@ -2994,7 +3211,7 @@
       <c r="F39" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="H39" s="88" t="s">
+      <c r="H39" s="85" t="s">
         <v>78</v>
       </c>
       <c r="I39" s="83"/>
@@ -3023,9 +3240,15 @@
       </c>
     </row>
     <row r="41" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="4"/>
+      <c r="A41" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" s="7">
+        <v>45553</v>
+      </c>
+      <c r="C41" s="4">
+        <v>3510.6</v>
+      </c>
       <c r="E41" s="4"/>
       <c r="F41" s="33"/>
       <c r="H41" s="44" t="s">
@@ -3036,13 +3259,20 @@
       </c>
       <c r="J41" s="73">
         <f>I41-I47</f>
-        <v>12000</v>
+        <v>5184.3999999999996</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="7"/>
+      <c r="A42" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" s="7">
+        <v>45555</v>
+      </c>
       <c r="C42" s="4"/>
+      <c r="D42">
+        <v>2280</v>
+      </c>
       <c r="E42" s="4"/>
       <c r="F42" s="33"/>
       <c r="H42" s="44" t="s">
@@ -3053,13 +3283,19 @@
       </c>
       <c r="J42" s="73">
         <f>I42-I48</f>
-        <v>15000</v>
+        <v>9970</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="4"/>
+      <c r="A43" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" s="7">
+        <v>45560</v>
+      </c>
+      <c r="C43" s="4">
+        <v>3305</v>
+      </c>
       <c r="E43" s="4"/>
       <c r="F43" s="33"/>
       <c r="H43" s="44" t="s">
@@ -3074,9 +3310,16 @@
       </c>
     </row>
     <row r="44" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="7"/>
+      <c r="A44" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B44" s="7">
+        <v>45562</v>
+      </c>
       <c r="C44" s="4"/>
+      <c r="D44">
+        <v>2750</v>
+      </c>
       <c r="E44" s="4"/>
       <c r="F44" s="33"/>
       <c r="H44" s="40" t="s">
@@ -3095,11 +3338,11 @@
       <c r="B45" s="20"/>
       <c r="C45" s="67">
         <f>SUM(C40:C44)</f>
-        <v>0</v>
+        <v>6815.6</v>
       </c>
       <c r="D45" s="67">
         <f>SUM(D40:D44)</f>
-        <v>0</v>
+        <v>5030</v>
       </c>
       <c r="E45" s="21">
         <f>SUM(E40:E44)</f>
@@ -3128,7 +3371,7 @@
       </c>
       <c r="I47" s="74">
         <f>C45</f>
-        <v>0</v>
+        <v>6815.6</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
@@ -3137,7 +3380,7 @@
       </c>
       <c r="I48" s="74">
         <f>D45</f>
-        <v>0</v>
+        <v>5030</v>
       </c>
     </row>
     <row r="49" spans="8:9" x14ac:dyDescent="0.2">
@@ -3155,7 +3398,7 @@
       </c>
       <c r="I50" s="75">
         <f>I47+I49+I48</f>
-        <v>492.91</v>
+        <v>12338.51</v>
       </c>
     </row>
     <row r="51" spans="8:9" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
@@ -3165,17 +3408,14 @@
       </c>
       <c r="I52" s="37">
         <f>I44-I50</f>
-        <v>31507.09</v>
+        <v>19661.489999999998</v>
       </c>
     </row>
     <row r="53" spans="8:9" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A37:G38"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="I26:J26"/>
+  <mergeCells count="15">
+    <mergeCell ref="AB3:AD3"/>
+    <mergeCell ref="W3:Y3"/>
     <mergeCell ref="A1:G2"/>
     <mergeCell ref="M3:O3"/>
     <mergeCell ref="R3:T3"/>
@@ -3184,6 +3424,11 @@
     <mergeCell ref="A16:G17"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="I4:J4"/>
+    <mergeCell ref="A37:G38"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="I26:J26"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>